<commit_message>
Sube archivo con encuesta ficticia
</commit_message>
<xml_diff>
--- a/data/encuesta.xlsx
+++ b/data/encuesta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\R\Club_de_R\r4hr_microaprendizajes\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76270C16-2F6C-4626-B844-074FF9C6DC4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDF9A89-A449-4A9A-A2D9-0D3876AB9AD8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -132,10 +132,6 @@
     <t>Togo</t>
   </si>
   <si>
-    <t xml:space="preserve">Los líderes son unos capos
-</t>
-  </si>
-  <si>
     <t>Que grosso es trabajar acá</t>
   </si>
   <si>
@@ -146,6 +142,9 @@
   </si>
   <si>
     <t>Una pregunta con un texto muy pero muy pero muy largo, de verdad que es muy muy muy largo</t>
+  </si>
+  <si>
+    <t>Los líderes son unos capos</t>
   </si>
 </sst>
 </file>
@@ -181,10 +180,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -248,7 +248,7 @@
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Tu cargo/nivel:" dataDxfId="5"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Una pregunta con un texto muy pero muy pero muy largo, de verdad que es muy muy muy largo" dataDxfId="4"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Otra pregunta que tiene muchísimo texto escrito en la encuesta y quedó tan larga que no entra en un solo renglón y que me hace preguntarme cómo la voy a poner en un gráfico" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Los líderes son unos capos_x000a_" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Los líderes son unos capos" dataDxfId="2"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Que grosso es trabajar acá" dataDxfId="1"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Esta encuesta es genial" dataDxfId="0"/>
   </tableColumns>
@@ -555,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K655"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,19 +587,19 @@
         <v>2</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -627,7 +627,7 @@
       <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="J2" s="1" t="s">

</xml_diff>